<commit_message>
Changed logic of excel
</commit_message>
<xml_diff>
--- a/Warehouse/Resources/Template.xlsx
+++ b/Warehouse/Resources/Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Производственная практика\Warehouse\Warehouse\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D0F3189-6E49-4DE7-9F94-7235C858C3F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B47FB97-924B-4D54-9C25-DD39B7B4EBC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" activeTab="-1"/>
   </bookViews>
@@ -20,9 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
-  <si>
-    <t>Реестр документов по поступлению</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+  <si>
+    <t>Отчёт о движении продуктов</t>
+  </si>
+  <si>
+    <t>Период: 2023-10-14 - 2023-10-29</t>
   </si>
   <si>
     <t>Номер заказа</t>
@@ -144,11 +147,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyProtection="1"/>
   </cellXfs>
@@ -465,7 +471,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -508,119 +514,152 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="D4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="E4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="F4" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="3" t="s">
+      <c r="G4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="3" t="s">
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="C5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="D5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="E5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="F5" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="s">
+      <c r="G5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="3" t="s">
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="C6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="E6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="F6" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="3" t="s">
+      <c r="G6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="3" t="s">
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="3" t="s">
+      <c r="B7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="3" t="s">
+      <c r="F7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="3" t="s">
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="B8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="3" t="s">
+      <c r="E8" s="4" t="s">
         <v>27</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
   <mergeCells>
     <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:G2"/>
   </mergeCells>
   <pageSetup orientation="landscape"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Completed logic of product flow report
</commit_message>
<xml_diff>
--- a/Warehouse/Resources/Template.xlsx
+++ b/Warehouse/Resources/Template.xlsx
@@ -20,12 +20,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Отчёт о движении продуктов</t>
   </si>
   <si>
-    <t>Период: 2023-10-14 - 2023-10-29</t>
+    <t>Период: 2023-10-07 - 2023-10-29</t>
+  </si>
+  <si>
+    <t>ОАО Гомельский Мясокомбинат</t>
+  </si>
+  <si>
+    <t>Адрес: Гомель, ул. Ильича, 2</t>
   </si>
   <si>
     <t>Номер заказа</t>
@@ -471,7 +477,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -533,133 +539,182 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>8</v>
+      <c r="B4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>15</v>
-      </c>
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="4" t="s">
+      <c r="E9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="4" t="s">
+    </row>
+    <row r="10">
+      <c r="A10" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" s="4" t="s">
+      <c r="B10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>28</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <mergeCells>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A5:G5"/>
   </mergeCells>
   <pageSetup orientation="landscape"/>
   <headerFooter/>

</xml_diff>